<commit_message>
maj feuille 11 inovcom
</commit_message>
<xml_diff>
--- a/Inovcomserveur.xlsx
+++ b/Inovcomserveur.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Felana reporting\Automatisation-reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\01421\Automatisation-reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DBA008-939A-459F-B0B8-00E71CDE3600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1245" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1245" windowWidth="29040" windowHeight="15840" tabRatio="772" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
     <sheet name="Feuil14" sheetId="14" r:id="rId13"/>
     <sheet name="Feuil13" sheetId="13" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -760,7 +759,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -783,7 +782,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -808,6 +807,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -821,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -835,11 +840,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1153,7 +1160,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -1308,7 +1315,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -1411,18 +1418,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil11"/>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="3" width="68.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" customWidth="1"/>
     <col min="5" max="5" width="27.140625" customWidth="1"/>
     <col min="6" max="6" width="33.5703125" customWidth="1"/>
@@ -1432,388 +1440,388 @@
     <col min="10" max="11" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="5">
-        <v>0</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="17">
+        <v>0</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="5">
-        <v>0</v>
-      </c>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="17">
+        <v>0</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="17" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="17">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="17">
+        <v>0</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="17" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="17">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="17" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="18">
+        <v>0</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="10" t="s">
+      <c r="H4" s="17">
+        <v>0</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="17" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="17">
         <v>1</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="17">
+        <v>0</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="17" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="17">
+        <v>0</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="17" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="17">
+        <v>0</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="17" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="H8" s="17">
+        <v>0</v>
+      </c>
+      <c r="I8" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="17" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5" t="s">
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="I9" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="17" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="17">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="s">
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="I10" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="17" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="17">
         <v>1</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5" t="s">
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="17" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1876,7 +1884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil12"/>
   <dimension ref="A1:K7"/>
   <sheetViews>
@@ -2116,7 +2124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E046DF-6906-4894-91CC-F871F4CD6A27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil14"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -2202,7 +2210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF15B2A4-2E15-464A-8C17-EC87886F15CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil13"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -2215,7 +2223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
@@ -2834,7 +2842,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K17">
+  <sortState ref="A2:K17">
     <sortCondition ref="A1:A17"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2844,12 +2852,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2998,7 +3006,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -3235,7 +3243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:L35"/>
   <sheetViews>
@@ -3309,7 +3317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil6"/>
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -3367,7 +3375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil7"/>
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -3390,79 +3398,79 @@
     <col min="12" max="12" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="14">
-        <v>0</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="13">
+        <v>0</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="14">
-        <v>0</v>
-      </c>
-      <c r="I1" s="14" t="s">
+      <c r="H1" s="13">
+        <v>0</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="16">
-        <v>0</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="15">
+        <v>0</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="16">
-        <v>0</v>
-      </c>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="15">
+        <v>0</v>
+      </c>
+      <c r="I2" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3472,7 +3480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil8"/>
   <dimension ref="A1:J20"/>
   <sheetViews>
@@ -3569,7 +3577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil10"/>
   <dimension ref="A1:J1"/>
   <sheetViews>

</xml_diff>